<commit_message>
Ajustes para calcular el precio a la salida de la visita
</commit_message>
<xml_diff>
--- a/Requerimientos.xlsx
+++ b/Requerimientos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\Parqueadero\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D208D6AE-C25D-4171-B167-78B88D76497B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580CDF00-9CEC-426E-83C6-1DEF1BF4478F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -593,102 +593,102 @@
   </cellStyleXfs>
   <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1260,568 +1260,656 @@
   <dimension ref="A1:AMK25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="E24" sqref="E24:F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="36.5703125" style="15" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="15"/>
-    <col min="4" max="4" width="49.5703125" style="15" customWidth="1"/>
-    <col min="5" max="9" width="11.42578125" style="15"/>
-    <col min="10" max="10" width="37.140625" style="15" customWidth="1"/>
-    <col min="11" max="1025" width="11.42578125" style="15"/>
+    <col min="1" max="1" width="15.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="1"/>
+    <col min="4" max="4" width="49.5703125" style="1" customWidth="1"/>
+    <col min="5" max="9" width="11.42578125" style="1"/>
+    <col min="10" max="10" width="37.140625" style="1" customWidth="1"/>
+    <col min="11" max="1025" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="13" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="11" t="s">
+      <c r="B2" s="24"/>
+      <c r="C2" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="10" t="s">
+      <c r="D2" s="25"/>
+      <c r="E2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="9" t="s">
+      <c r="F2" s="26"/>
+      <c r="G2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="8" t="s">
+      <c r="H2" s="27"/>
+      <c r="I2" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="8"/>
-      <c r="K2" s="7" t="s">
+      <c r="J2" s="28"/>
+      <c r="K2" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="7"/>
+      <c r="L2" s="29"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="30"/>
+      <c r="C3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="3" t="s">
+      <c r="D3" s="31"/>
+      <c r="E3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="G3" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="2" t="s">
+      <c r="H3" s="32"/>
+      <c r="I3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="4" t="s">
+      <c r="J3" s="14"/>
+      <c r="K3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="4"/>
+      <c r="L3" s="9"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="17" t="s">
+      <c r="B4" s="21"/>
+      <c r="C4" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="18" t="s">
+      <c r="D4" s="33"/>
+      <c r="E4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="18"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="2" t="s">
+      <c r="F4" s="7"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="2"/>
-      <c r="K4" s="4" t="s">
+      <c r="J4" s="14"/>
+      <c r="K4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="4"/>
+      <c r="L4" s="9"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="19" t="s">
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="20"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="21" t="s">
+      <c r="D5" s="6"/>
+      <c r="E5" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="21"/>
-      <c r="K5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="L5" s="4"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" s="9"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="22" t="s">
+      <c r="A6" s="21"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="20"/>
-      <c r="G6" s="23" t="s">
+      <c r="D6" s="15"/>
+      <c r="E6" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="19"/>
+      <c r="G6" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="23"/>
-      <c r="I6" s="2" t="s">
+      <c r="H6" s="20"/>
+      <c r="I6" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="2"/>
-      <c r="K6" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="L6" s="18"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" s="7"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="24" t="s">
+      <c r="B7" s="21"/>
+      <c r="C7" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="18" t="s">
+      <c r="D7" s="18"/>
+      <c r="E7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="2" t="s">
+      <c r="F7" s="7"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="J7" s="2"/>
-      <c r="K7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="L7" s="4"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="L7" s="9"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="24" t="s">
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="24"/>
-      <c r="E8" s="20" t="s">
+      <c r="D8" s="18"/>
+      <c r="E8" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="2" t="s">
+      <c r="F8" s="19"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="J8" s="2"/>
-      <c r="K8" s="4" t="s">
+      <c r="J8" s="14"/>
+      <c r="K8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="L8" s="4"/>
+      <c r="L8" s="9"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="19" t="s">
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="19"/>
-      <c r="E9" s="4" t="s">
+      <c r="D9" s="6"/>
+      <c r="E9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="2" t="s">
+      <c r="F9" s="9"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="2"/>
-      <c r="K9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="L9" s="4"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="L9" s="9"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="24" t="s">
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="20"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="2" t="s">
+      <c r="D10" s="18"/>
+      <c r="E10" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="19"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="J10" s="2"/>
-      <c r="K10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="L10" s="4"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="L10" s="9"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="24" t="s">
+      <c r="A11" s="21"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="24"/>
-      <c r="E11" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="2" t="s">
+      <c r="D11" s="18"/>
+      <c r="E11" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="19"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="J11" s="2"/>
-      <c r="K11" s="4" t="s">
+      <c r="J11" s="14"/>
+      <c r="K11" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="L11" s="9"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="21"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="18"/>
+      <c r="E12" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="19"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="J12" s="14"/>
+      <c r="K12" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="L12" s="9"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="9"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="J13" s="14"/>
+      <c r="K13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="21"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="9"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="J14" s="14"/>
+      <c r="K14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="L14" s="9"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="9"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="J15" s="14"/>
+      <c r="K15" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="L15" s="9"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="21"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="9"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="J16" s="14"/>
+      <c r="K16" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="L16" s="17"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="9"/>
+      <c r="G17" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="H17" s="12"/>
+      <c r="I17" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="J17" s="13"/>
+      <c r="K17" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="L17" s="9"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="21"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="9"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="J18" s="14"/>
+      <c r="K18" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="L11" s="4"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="24"/>
-      <c r="E12" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="20"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J12" s="2"/>
-      <c r="K12" s="4" t="s">
+      <c r="L18" s="9"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="9"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="J19" s="14"/>
+      <c r="K19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="L19" s="9"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="21"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="15"/>
+      <c r="E20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="9"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="J20" s="16"/>
+      <c r="K20" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="L20" s="11"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="6"/>
+      <c r="E21" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="7"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="6"/>
+      <c r="E22" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="L12" s="4"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J13" s="2"/>
-      <c r="K13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="L13" s="4"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J14" s="2"/>
-      <c r="K14" s="4" t="s">
+      <c r="F22" s="9"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="L14" s="4"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J15" s="2"/>
-      <c r="K15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="L15" s="4"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J16" s="2"/>
-      <c r="K16" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="L16" s="25"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="19"/>
-      <c r="E17" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="H17" s="26"/>
-      <c r="I17" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="J17" s="27"/>
-      <c r="K17" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="L17" s="4"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="19"/>
-      <c r="E18" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J18" s="2"/>
-      <c r="K18" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="L18" s="4"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="19"/>
-      <c r="E19" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="J19" s="2"/>
-      <c r="K19" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="L19" s="4"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" s="22"/>
-      <c r="E20" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="J20" s="28"/>
-      <c r="K20" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="L20" s="29"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="30"/>
-      <c r="C21" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F21" s="18"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="32"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="30"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" s="19"/>
-      <c r="E22" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22" s="4"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="32"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="30"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" s="19"/>
-      <c r="E23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="4"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="31"/>
-      <c r="I23" s="32"/>
-      <c r="J23" s="32"/>
-      <c r="K23" s="33"/>
-      <c r="L23" s="33"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="30"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="19" t="s">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="19"/>
-      <c r="E24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F24" s="4"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="32"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="33"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="9"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="30"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="34" t="s">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="34"/>
-      <c r="E25" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" s="29"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="32"/>
-      <c r="J25" s="32"/>
-      <c r="K25" s="33"/>
-      <c r="L25" s="33"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="11"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="112">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G1:L1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H5"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="A4:B6"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H16"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="A7:B20"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H20"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="K20:L20"/>
     <mergeCell ref="I25:J25"/>
     <mergeCell ref="K25:L25"/>
     <mergeCell ref="A21:B25"/>
@@ -1846,94 +1934,6 @@
     <mergeCell ref="I24:J24"/>
     <mergeCell ref="K24:L24"/>
     <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H20"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H16"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="A7:B20"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="G1:L1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H5"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="A4:B6"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="C6:D6"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:F25">
     <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="Finalizado"/>

</xml_diff>

<commit_message>
Ajustes varios en el menú de administrador y en la entrada y salida de vehiculos. Se añaden tablas y se modifican algunas en la base de datos
</commit_message>
<xml_diff>
--- a/Requerimientos.xlsx
+++ b/Requerimientos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\Parqueadero\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580CDF00-9CEC-426E-83C6-1DEF1BF4478F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC95512-1779-40FD-BDDD-11993D1ED6A6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -595,6 +595,90 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -604,91 +688,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1260,7 +1260,7 @@
   <dimension ref="A1:AMK25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24:F24"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1275,553 +1275,641 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="23" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="25" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="26" t="s">
+      <c r="D2" s="6"/>
+      <c r="E2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="26"/>
-      <c r="G2" s="27" t="s">
+      <c r="F2" s="7"/>
+      <c r="G2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="27"/>
-      <c r="I2" s="28" t="s">
+      <c r="H2" s="8"/>
+      <c r="I2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="28"/>
-      <c r="K2" s="29" t="s">
+      <c r="J2" s="9"/>
+      <c r="K2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="29"/>
+      <c r="L2" s="10"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="31" t="s">
+      <c r="B3" s="11"/>
+      <c r="C3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="32" t="s">
+      <c r="D3" s="12"/>
+      <c r="E3" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="13"/>
+      <c r="G3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="32"/>
-      <c r="I3" s="14" t="s">
+      <c r="H3" s="14"/>
+      <c r="I3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="14"/>
-      <c r="K3" s="9" t="s">
+      <c r="J3" s="15"/>
+      <c r="K3" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="13"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="16"/>
+      <c r="C4" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="17"/>
+      <c r="E4" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="18"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="15"/>
+      <c r="K4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="13"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="E5" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="20"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="21"/>
+      <c r="K5" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" s="13"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="22"/>
+      <c r="E6" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="20"/>
+      <c r="G6" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="23"/>
+      <c r="I6" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="15"/>
+      <c r="K6" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" s="18"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="16"/>
+      <c r="C7" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="24"/>
+      <c r="E7" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="18"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="15"/>
+      <c r="K7" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L7" s="13"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="24"/>
+      <c r="E8" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="20"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" s="15"/>
+      <c r="K8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="9"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" s="14"/>
-      <c r="K4" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L4" s="9"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="34"/>
-      <c r="K5" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="L5" s="9"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="20"/>
-      <c r="I6" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" s="14"/>
-      <c r="K6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="L6" s="7"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" s="14"/>
-      <c r="K7" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="L7" s="9"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="19"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="J8" s="14"/>
-      <c r="K8" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="L8" s="9"/>
+      <c r="L8" s="13"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="6" t="s">
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="14" t="s">
+      <c r="D9" s="19"/>
+      <c r="E9" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="13"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="14"/>
-      <c r="K9" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="L9" s="9"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L9" s="13"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="18" t="s">
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="19"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="14" t="s">
+      <c r="D10" s="24"/>
+      <c r="E10" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="20"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="J10" s="14"/>
-      <c r="K10" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="L10" s="9"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L10" s="13"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="18" t="s">
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="19"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="14" t="s">
+      <c r="D11" s="24"/>
+      <c r="E11" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="20"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="J11" s="14"/>
-      <c r="K11" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="L11" s="9"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L11" s="13"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="18" t="s">
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="19"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="14" t="s">
+      <c r="D12" s="24"/>
+      <c r="E12" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="20"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="J12" s="14"/>
-      <c r="K12" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="L12" s="9"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L12" s="13"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="6" t="s">
+      <c r="A13" s="16"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="14" t="s">
+      <c r="D13" s="19"/>
+      <c r="E13" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="13"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="14"/>
-      <c r="K13" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="L13" s="9"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L13" s="13"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="6" t="s">
+      <c r="A14" s="16"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="14" t="s">
+      <c r="D14" s="19"/>
+      <c r="E14" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="13"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="J14" s="14"/>
-      <c r="K14" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="L14" s="9"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L14" s="13"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="6" t="s">
+      <c r="A15" s="16"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="14" t="s">
+      <c r="D15" s="19"/>
+      <c r="E15" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="13"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="J15" s="14"/>
-      <c r="K15" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="L15" s="9"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L15" s="13"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="6" t="s">
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="9"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="14" t="s">
+      <c r="D16" s="19"/>
+      <c r="E16" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="13"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="J16" s="14"/>
-      <c r="K16" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="L16" s="17"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="L16" s="25"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="6" t="s">
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="9"/>
-      <c r="G17" s="12" t="s">
+      <c r="D17" s="19"/>
+      <c r="E17" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="13"/>
+      <c r="G17" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="H17" s="12"/>
-      <c r="I17" s="13" t="s">
+      <c r="H17" s="28"/>
+      <c r="I17" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="J17" s="13"/>
-      <c r="K17" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="L17" s="9"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L17" s="13"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="6" t="s">
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="9"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="14" t="s">
+      <c r="D18" s="19"/>
+      <c r="E18" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="13"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="J18" s="14"/>
-      <c r="K18" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="L18" s="9"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L18" s="13"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="6" t="s">
+      <c r="A19" s="16"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="9"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="14" t="s">
+      <c r="D19" s="19"/>
+      <c r="E19" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="13"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="J19" s="14"/>
-      <c r="K19" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="L19" s="9"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L19" s="13"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="15" t="s">
+      <c r="A20" s="16"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="15"/>
-      <c r="E20" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="9"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="16" t="s">
+      <c r="D20" s="22"/>
+      <c r="E20" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="13"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="J20" s="16"/>
-      <c r="K20" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="L20" s="11"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="L20" s="26"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="6" t="s">
+      <c r="B21" s="33"/>
+      <c r="C21" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F21" s="7"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="18"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="32"/>
+      <c r="L21" s="32"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="6" t="s">
+      <c r="A22" s="33"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22" s="9"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="13"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="32"/>
+      <c r="L22" s="32"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="6" t="s">
+      <c r="A23" s="33"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="9"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="13"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="32"/>
+      <c r="L23" s="32"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="6" t="s">
+      <c r="A24" s="33"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="13"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="32"/>
+      <c r="L24" s="32"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="10" t="s">
+      <c r="A25" s="33"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="10"/>
-      <c r="E25" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" s="11"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="26"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="31"/>
+      <c r="J25" s="31"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="112">
+    <mergeCell ref="A21:B25"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H20"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H16"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="A7:B20"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="I11:J11"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="G1:L1"/>
     <mergeCell ref="A2:B2"/>
@@ -1846,94 +1934,6 @@
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="K5:L5"/>
     <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H16"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="A7:B20"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H20"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="A21:B25"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="C25:D25"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:F25">
     <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="Finalizado"/>

</xml_diff>